<commit_message>
infrastructure availability data developed
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_HeatingTechnology.xlsx
+++ b/projects/test_building/input/ID_HeatingTechnology.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04973F62-132C-8E4B-B118-854E3FD29529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,11 +155,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0">
+  <autoFilter ref="A1:B26"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_heating_technology"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
+    <tableColumn id="1" name="id_heating_technology"/>
+    <tableColumn id="2" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,20 +427,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -449,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -457,7 +456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21</v>
       </c>
@@ -465,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22</v>
       </c>
@@ -473,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23</v>
       </c>
@@ -481,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24</v>
       </c>
@@ -489,7 +488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -497,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>26</v>
       </c>
@@ -505,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -513,7 +512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
@@ -521,7 +520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>29</v>
       </c>
@@ -529,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>210</v>
       </c>
@@ -537,7 +536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>211</v>
       </c>
@@ -545,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>212</v>
       </c>
@@ -553,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>213</v>
       </c>
@@ -561,7 +560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31</v>
       </c>
@@ -569,7 +568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32</v>
       </c>
@@ -577,7 +576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
@@ -585,7 +584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>34</v>
       </c>
@@ -593,7 +592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>41</v>
       </c>
@@ -601,7 +600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>42</v>
       </c>
@@ -609,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>43</v>
       </c>
@@ -617,7 +616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>44</v>
       </c>
@@ -625,7 +624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>45</v>
       </c>
@@ -633,7 +632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>46</v>
       </c>
@@ -641,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>50</v>
       </c>

</xml_diff>